<commit_message>
Added years of speeches to the Team Roles document
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pitt-my.sharepoint.com/personal/tps30_pitt_edu/Documents/Year 3 - Semester 2/Digital Humanities/Inaug Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="8_{8B435B98-D5CA-3C4C-A843-9352383D35BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{657B00D8-CCDF-C94C-A791-C46C9EBA0746}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D5B66F2-D78D-A64B-9851-869483E5BC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="15700" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16820" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$C$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>Term</t>
   </si>
@@ -123,6 +123,9 @@
   </si>
   <si>
     <t>Joe Biden</t>
+  </si>
+  <si>
+    <t>Year</t>
   </si>
 </sst>
 </file>
@@ -486,427 +489,539 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
-  <dimension ref="A1:C37"/>
+  <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
-        <v>1</v>
+        <v>28</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1901</v>
+      </c>
+      <c r="B2" t="s">
         <v>4</v>
       </c>
-      <c r="B2">
-        <v>2</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1901</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3">
-        <v>1</v>
-      </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1905</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4">
-        <v>2</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1909</v>
+      </c>
+      <c r="B5" t="s">
         <v>8</v>
       </c>
-      <c r="B5">
-        <v>1</v>
-      </c>
-      <c r="C5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1913</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1917</v>
+      </c>
+      <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1921</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="C8">
+        <v>1</v>
+      </c>
+      <c r="D8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1923</v>
+      </c>
+      <c r="B9" t="s">
         <v>11</v>
       </c>
-      <c r="B9">
-        <v>1</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1925</v>
+      </c>
+      <c r="B10" t="s">
         <v>11</v>
       </c>
-      <c r="B10">
-        <v>2</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+      <c r="C10">
+        <v>2</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1929</v>
+      </c>
+      <c r="B11" t="s">
         <v>12</v>
       </c>
-      <c r="B11">
-        <v>1</v>
-      </c>
-      <c r="C11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1933</v>
+      </c>
+      <c r="B12" t="s">
         <v>13</v>
       </c>
-      <c r="B12">
-        <v>1</v>
-      </c>
-      <c r="C12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1937</v>
+      </c>
+      <c r="B13" t="s">
         <v>13</v>
       </c>
-      <c r="B13">
-        <v>2</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
+      <c r="C13">
+        <v>2</v>
+      </c>
+      <c r="D13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1941</v>
+      </c>
+      <c r="B14" t="s">
         <v>13</v>
       </c>
-      <c r="B14">
+      <c r="C14">
         <v>3</v>
       </c>
-      <c r="C14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="D14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1945</v>
+      </c>
+      <c r="B15" t="s">
         <v>13</v>
       </c>
-      <c r="B15">
+      <c r="C15">
         <v>4</v>
       </c>
-      <c r="C15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
+      <c r="D15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1945</v>
+      </c>
+      <c r="B16" t="s">
         <v>14</v>
       </c>
-      <c r="B16">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
+      <c r="C16">
+        <v>1</v>
+      </c>
+      <c r="D16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17">
+        <v>1949</v>
+      </c>
+      <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="B17">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
+      <c r="C17">
+        <v>2</v>
+      </c>
+      <c r="D17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18">
+        <v>1953</v>
+      </c>
+      <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="B18">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A19">
+        <v>1957</v>
+      </c>
+      <c r="B19" t="s">
         <v>15</v>
       </c>
-      <c r="B19">
-        <v>2</v>
-      </c>
-      <c r="C19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
+      <c r="C19">
+        <v>2</v>
+      </c>
+      <c r="D19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1961</v>
+      </c>
+      <c r="B20" t="s">
         <v>16</v>
       </c>
-      <c r="B20">
-        <v>1</v>
-      </c>
-      <c r="C20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
+      <c r="C20">
+        <v>1</v>
+      </c>
+      <c r="D20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1963</v>
+      </c>
+      <c r="B21" t="s">
         <v>17</v>
       </c>
-      <c r="B21">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
+      <c r="C21">
+        <v>1</v>
+      </c>
+      <c r="D21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1965</v>
+      </c>
+      <c r="B22" t="s">
         <v>17</v>
       </c>
-      <c r="B22">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
+      <c r="C22">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1969</v>
+      </c>
+      <c r="B23" t="s">
         <v>18</v>
       </c>
-      <c r="B23">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1973</v>
+      </c>
+      <c r="B24" t="s">
         <v>18</v>
       </c>
-      <c r="B24">
-        <v>2</v>
-      </c>
-      <c r="C24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
+      <c r="C24">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1974</v>
+      </c>
+      <c r="B25" t="s">
         <v>19</v>
       </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
+      <c r="C25">
+        <v>1</v>
+      </c>
+      <c r="D25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1977</v>
+      </c>
+      <c r="B26" t="s">
         <v>20</v>
       </c>
-      <c r="B26">
-        <v>1</v>
-      </c>
-      <c r="C26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1981</v>
+      </c>
+      <c r="B27" t="s">
         <v>21</v>
       </c>
-      <c r="B27">
-        <v>1</v>
-      </c>
-      <c r="C27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1985</v>
+      </c>
+      <c r="B28" t="s">
         <v>21</v>
       </c>
-      <c r="B28">
-        <v>2</v>
-      </c>
-      <c r="C28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
+      <c r="C28">
+        <v>2</v>
+      </c>
+      <c r="D28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1989</v>
+      </c>
+      <c r="B29" t="s">
         <v>22</v>
       </c>
-      <c r="B29">
-        <v>1</v>
-      </c>
-      <c r="C29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1993</v>
+      </c>
+      <c r="B30" t="s">
         <v>23</v>
       </c>
-      <c r="B30">
-        <v>1</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
+      <c r="C30">
+        <v>1</v>
+      </c>
+      <c r="D30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1997</v>
+      </c>
+      <c r="B31" t="s">
         <v>23</v>
       </c>
-      <c r="B31">
-        <v>2</v>
-      </c>
-      <c r="C31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>2001</v>
+      </c>
+      <c r="B32" t="s">
         <v>24</v>
       </c>
-      <c r="B32">
-        <v>1</v>
-      </c>
-      <c r="C32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
+      <c r="C32">
+        <v>1</v>
+      </c>
+      <c r="D32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>2005</v>
+      </c>
+      <c r="B33" t="s">
         <v>24</v>
       </c>
-      <c r="B33">
-        <v>2</v>
-      </c>
-      <c r="C33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>2009</v>
+      </c>
+      <c r="B34" t="s">
         <v>25</v>
       </c>
-      <c r="B34">
-        <v>1</v>
-      </c>
-      <c r="C34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>2013</v>
+      </c>
+      <c r="B35" t="s">
         <v>25</v>
       </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
+      <c r="C35">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>2017</v>
+      </c>
+      <c r="B36" t="s">
         <v>26</v>
       </c>
-      <c r="B36">
-        <v>1</v>
-      </c>
-      <c r="C36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
+      <c r="C36">
+        <v>1</v>
+      </c>
+      <c r="D36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>2021</v>
+      </c>
+      <c r="B37" t="s">
         <v>27</v>
       </c>
-      <c r="B37">
-        <v>1</v>
-      </c>
-      <c r="C37" t="s">
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
+  <autoFilter ref="B1:D37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Assigned ID numbers to each speech in the Team Roles document
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D5B66F2-D78D-A64B-9851-869483E5BC32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B0C344-8BCE-F04D-A08B-DCCD5733FE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="16820" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="20120" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$D$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
   <si>
     <t>Term</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Year</t>
+  </si>
+  <si>
+    <t>ID</t>
   </si>
 </sst>
 </file>
@@ -169,12 +172,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -489,539 +493,649 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
-  <dimension ref="A1:D37"/>
+  <dimension ref="A1:E37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" customWidth="1"/>
-    <col min="2" max="2" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.33203125" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="3">
+        <v>1</v>
+      </c>
+      <c r="B2">
         <v>1901</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-      <c r="D2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3">
         <v>1901</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C3">
-        <v>1</v>
-      </c>
-      <c r="D3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4">
         <v>1905</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4">
-        <v>2</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5">
         <v>1909</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>8</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D5">
+        <v>1</v>
+      </c>
+      <c r="E5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6">
         <v>1913</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>9</v>
       </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
         <v>1917</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>9</v>
       </c>
-      <c r="C7">
-        <v>2</v>
-      </c>
-      <c r="D7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
         <v>1921</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>10</v>
       </c>
-      <c r="C8">
-        <v>1</v>
-      </c>
-      <c r="D8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="3">
+        <v>8</v>
+      </c>
+      <c r="B9">
         <v>1923</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>11</v>
       </c>
-      <c r="C9">
-        <v>1</v>
-      </c>
-      <c r="D9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
         <v>1925</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>11</v>
       </c>
-      <c r="C10">
-        <v>2</v>
-      </c>
-      <c r="D10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D10">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
         <v>1929</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>12</v>
       </c>
-      <c r="C11">
-        <v>1</v>
-      </c>
-      <c r="D11" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
         <v>1933</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>13</v>
       </c>
-      <c r="C12">
-        <v>1</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D12">
+        <v>1</v>
+      </c>
+      <c r="E12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
         <v>1937</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>13</v>
       </c>
-      <c r="C13">
-        <v>2</v>
-      </c>
-      <c r="D13" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
         <v>1941</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>13</v>
       </c>
-      <c r="C14">
+      <c r="D14">
         <v>3</v>
       </c>
-      <c r="D14" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
         <v>1945</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>13</v>
       </c>
-      <c r="C15">
+      <c r="D15">
         <v>4</v>
       </c>
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="E15" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3">
+        <v>15</v>
+      </c>
+      <c r="B16">
         <v>1945</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>14</v>
       </c>
-      <c r="C16">
-        <v>1</v>
-      </c>
-      <c r="D16" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="D16">
+        <v>1</v>
+      </c>
+      <c r="E16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>16</v>
+      </c>
+      <c r="B17">
         <v>1949</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>14</v>
       </c>
-      <c r="C17">
-        <v>2</v>
-      </c>
-      <c r="D17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>2</v>
+      </c>
+      <c r="E17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18">
         <v>1953</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>15</v>
       </c>
-      <c r="C18">
-        <v>1</v>
-      </c>
-      <c r="D18" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>1</v>
+      </c>
+      <c r="E18" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19">
         <v>1957</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>15</v>
       </c>
-      <c r="C19">
-        <v>2</v>
-      </c>
-      <c r="D19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>2</v>
+      </c>
+      <c r="E19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20">
         <v>1961</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>16</v>
       </c>
-      <c r="C20">
-        <v>1</v>
-      </c>
-      <c r="D20" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>1</v>
+      </c>
+      <c r="E20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21">
         <v>1963</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>17</v>
       </c>
-      <c r="C21">
-        <v>1</v>
-      </c>
-      <c r="D21" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22">
         <v>1965</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>17</v>
       </c>
-      <c r="C22">
-        <v>2</v>
-      </c>
-      <c r="D22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23">
         <v>1969</v>
       </c>
-      <c r="B23" t="s">
+      <c r="C23" t="s">
         <v>18</v>
       </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="D23">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="3">
+        <v>23</v>
+      </c>
+      <c r="B24">
         <v>1973</v>
       </c>
-      <c r="B24" t="s">
+      <c r="C24" t="s">
         <v>18</v>
       </c>
-      <c r="C24">
-        <v>2</v>
-      </c>
-      <c r="D24" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25">
         <v>1974</v>
       </c>
-      <c r="B25" t="s">
+      <c r="C25" t="s">
         <v>19</v>
       </c>
-      <c r="C25">
-        <v>1</v>
-      </c>
-      <c r="D25" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>1</v>
+      </c>
+      <c r="E25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26">
         <v>1977</v>
       </c>
-      <c r="B26" t="s">
+      <c r="C26" t="s">
         <v>20</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>1</v>
+      </c>
+      <c r="E26" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27">
         <v>1981</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>21</v>
       </c>
-      <c r="C27">
-        <v>1</v>
-      </c>
-      <c r="D27" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>1</v>
+      </c>
+      <c r="E27" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28">
         <v>1985</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>21</v>
       </c>
-      <c r="C28">
-        <v>2</v>
-      </c>
-      <c r="D28" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>2</v>
+      </c>
+      <c r="E28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29">
         <v>1989</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>22</v>
       </c>
-      <c r="C29">
-        <v>1</v>
-      </c>
-      <c r="D29" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <v>1</v>
+      </c>
+      <c r="E29" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30">
         <v>1993</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>23</v>
       </c>
-      <c r="C30">
-        <v>1</v>
-      </c>
-      <c r="D30" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="3">
+        <v>30</v>
+      </c>
+      <c r="B31">
         <v>1997</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>23</v>
       </c>
-      <c r="C31">
-        <v>2</v>
-      </c>
-      <c r="D31" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A32">
+      <c r="D31">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="3">
+        <v>31</v>
+      </c>
+      <c r="B32">
         <v>2001</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>24</v>
       </c>
-      <c r="C32">
-        <v>1</v>
-      </c>
-      <c r="D32" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D32">
+        <v>1</v>
+      </c>
+      <c r="E32" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33">
         <v>2005</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>24</v>
       </c>
-      <c r="C33">
-        <v>2</v>
-      </c>
-      <c r="D33" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D33">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34">
         <v>2009</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>25</v>
       </c>
-      <c r="C34">
-        <v>1</v>
-      </c>
-      <c r="D34" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35">
         <v>2013</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>25</v>
       </c>
-      <c r="C35">
-        <v>2</v>
-      </c>
-      <c r="D35" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D35">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36">
         <v>2017</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>26</v>
       </c>
-      <c r="C36">
-        <v>1</v>
-      </c>
-      <c r="D36" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="D36">
+        <v>1</v>
+      </c>
+      <c r="E36" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37">
         <v>2021</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>27</v>
       </c>
-      <c r="C37">
-        <v>1</v>
-      </c>
-      <c r="D37" t="s">
+      <c r="D37">
+        <v>1</v>
+      </c>
+      <c r="E37" t="s">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:D37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
+  <autoFilter ref="A1:E37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Created status column on team roles spreadsheet
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B0C344-8BCE-F04D-A08B-DCCD5733FE22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9C305-F585-E647-8AFF-AE71E6FFAC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="20120" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$E$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$37</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
   <si>
     <t>Term</t>
   </si>
@@ -129,6 +129,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
@@ -172,13 +181,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -493,9 +505,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
-  <dimension ref="A1:E37"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -505,7 +519,7 @@
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -521,8 +535,11 @@
       <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -538,8 +555,11 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F2" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -555,8 +575,11 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F3" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -572,8 +595,11 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F4" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -589,8 +615,11 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F5" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -606,8 +635,11 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F6" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -623,8 +655,11 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F7" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -640,8 +675,11 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F8" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -657,8 +695,11 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F9" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -674,8 +715,11 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F10" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -691,8 +735,11 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F11" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -708,8 +755,11 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F12" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -725,8 +775,11 @@
       <c r="E13" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F13" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -742,8 +795,11 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F14" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -759,8 +815,11 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F15" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>15</v>
       </c>
@@ -776,8 +835,11 @@
       <c r="E16" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F16" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>16</v>
       </c>
@@ -793,8 +855,11 @@
       <c r="E17" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F17" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -810,8 +875,11 @@
       <c r="E18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F18" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -827,8 +895,11 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F19" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -844,8 +915,11 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F20" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -861,8 +935,11 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F21" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -878,8 +955,11 @@
       <c r="E22" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F22" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -895,8 +975,11 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F23" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>23</v>
       </c>
@@ -912,8 +995,11 @@
       <c r="E24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F24" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -929,8 +1015,11 @@
       <c r="E25" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F25" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -946,8 +1035,11 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F26" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -963,8 +1055,11 @@
       <c r="E27" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F27" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -980,8 +1075,11 @@
       <c r="E28" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F28" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -997,8 +1095,11 @@
       <c r="E29" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F29" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1014,8 +1115,11 @@
       <c r="E30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F30" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>30</v>
       </c>
@@ -1031,8 +1135,11 @@
       <c r="E31" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F31" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>31</v>
       </c>
@@ -1048,8 +1155,11 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F32" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1065,8 +1175,11 @@
       <c r="E33" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F33" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1082,8 +1195,11 @@
       <c r="E34" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F34" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1099,8 +1215,11 @@
       <c r="E35" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F35" s="4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1116,8 +1235,11 @@
       <c r="E36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F36" s="4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1133,9 +1255,12 @@
       <c r="E37" t="s">
         <v>7</v>
       </c>
+      <c r="F37" s="4" t="s">
+        <v>32</v>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:E37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
+  <autoFilter ref="A1:F37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated status on team roles
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1D9C305-F585-E647-8AFF-AE71E6FFAC89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B5B7E-8577-6A48-89DF-6EE5373BB4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="20120" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="18580" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Term</t>
   </si>
@@ -138,13 +138,16 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Sworn in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -156,6 +159,20 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF0070C0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC00000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -181,7 +198,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -189,7 +206,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -508,7 +531,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -575,8 +598,8 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>32</v>
+      <c r="F3" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -695,8 +718,8 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4" t="s">
-        <v>32</v>
+      <c r="F9" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -835,8 +858,8 @@
       <c r="E16" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="4" t="s">
-        <v>32</v>
+      <c r="F16" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
@@ -935,8 +958,8 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="4" t="s">
-        <v>32</v>
+      <c r="F21" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1015,8 +1038,8 @@
       <c r="E25" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="4" t="s">
-        <v>32</v>
+      <c r="F25" s="5" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1155,7 +1178,7 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="4" t="s">
+      <c r="F32" s="6" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1215,7 +1238,7 @@
       <c r="E35" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="4" t="s">
+      <c r="F35" s="6" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
team roles status update
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D2B5B7E-8577-6A48-89DF-6EE5373BB4FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180F6FCD-1905-7D4C-8242-80B9AD87C25A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18580" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
   <si>
     <t>Term</t>
   </si>
@@ -141,6 +141,9 @@
   </si>
   <si>
     <t>Sworn in</t>
+  </si>
+  <si>
+    <t>In Document</t>
   </si>
 </sst>
 </file>
@@ -531,7 +534,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -540,6 +543,7 @@
     <col min="2" max="2" width="8.6640625" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.33203125" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
@@ -659,7 +663,7 @@
         <v>6</v>
       </c>
       <c r="F6" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -779,7 +783,7 @@
         <v>6</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -839,7 +843,7 @@
         <v>6</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -899,7 +903,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
@@ -1019,7 +1023,7 @@
         <v>6</v>
       </c>
       <c r="F24" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
@@ -1079,7 +1083,7 @@
         <v>6</v>
       </c>
       <c r="F27" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
@@ -1139,7 +1143,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1199,7 +1203,7 @@
         <v>6</v>
       </c>
       <c r="F33" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
@@ -1259,7 +1263,7 @@
         <v>6</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Harding 1, Hoover 1, McKinley 2, Taft 1, Schema update, and team roles update
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4829667D-DBA1-6D47-A703-CCCF15294A8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E03EF1-884D-C84C-98C7-AD303A2A2B89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18580" windowHeight="15480" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
@@ -533,8 +533,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -582,8 +582,8 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
-        <v>32</v>
+      <c r="F2" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -642,8 +642,8 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>32</v>
+      <c r="F5" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
@@ -702,8 +702,8 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="4" t="s">
-        <v>32</v>
+      <c r="F8" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -762,8 +762,8 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="4" t="s">
-        <v>32</v>
+      <c r="F11" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -822,8 +822,8 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="4" t="s">
-        <v>32</v>
+      <c r="F14" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -882,8 +882,8 @@
       <c r="E17" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="4" t="s">
-        <v>32</v>
+      <c r="F17" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
@@ -942,8 +942,8 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="4" t="s">
-        <v>32</v>
+      <c r="F20" s="6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Nixon name fix and team roles update
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10116"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cde73a511afdd567/Documents/GitHub/Pres-Inaug-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="13_ncr:1_{40D60002-6B86-484B-A699-2C6FA77FF2B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{39ED2555-B110-4F3A-88E0-6046BABE1C8E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AE35E50-2741-214B-B7D3-522FE7961567}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="16000" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -241,10 +241,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -547,19 +543,19 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.59765625" customWidth="1"/>
-    <col min="2" max="2" width="8.59765625" customWidth="1"/>
-    <col min="3" max="3" width="17.09765625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.3984375" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>29</v>
       </c>
@@ -579,7 +575,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -599,7 +595,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -619,7 +615,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -639,7 +635,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>4</v>
       </c>
@@ -659,7 +655,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>5</v>
       </c>
@@ -679,7 +675,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>6</v>
       </c>
@@ -699,7 +695,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>7</v>
       </c>
@@ -719,7 +715,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>8</v>
       </c>
@@ -739,7 +735,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>9</v>
       </c>
@@ -759,7 +755,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>10</v>
       </c>
@@ -779,7 +775,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>11</v>
       </c>
@@ -799,7 +795,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>12</v>
       </c>
@@ -819,7 +815,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>13</v>
       </c>
@@ -839,7 +835,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>14</v>
       </c>
@@ -859,7 +855,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>15</v>
       </c>
@@ -879,7 +875,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>16</v>
       </c>
@@ -899,7 +895,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>17</v>
       </c>
@@ -919,7 +915,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>18</v>
       </c>
@@ -939,7 +935,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>19</v>
       </c>
@@ -959,7 +955,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>20</v>
       </c>
@@ -979,7 +975,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>21</v>
       </c>
@@ -999,7 +995,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1015,11 +1011,11 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F23" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1039,7 +1035,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1059,7 +1055,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1079,7 +1075,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1099,7 +1095,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1119,7 +1115,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1139,7 +1135,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1159,7 +1155,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1179,7 +1175,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1195,11 +1191,11 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="F32" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1219,7 +1215,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1239,7 +1235,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1259,7 +1255,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1279,7 +1275,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>36</v>
       </c>

</xml_diff>

<commit_message>
McKinley 2 and roles update
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taishanahan/Desktop/Pres-Inaug-Project/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A73EFAC-B8FF-7648-8E8C-2DF1060F3DFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5B4D661-F7B3-224A-8047-6913DF175298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="23260" windowHeight="16000" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="16060" windowHeight="15980" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -542,8 +542,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
   <dimension ref="A1:F37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="H30" sqref="H30"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -591,8 +591,8 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="5" t="s">
-        <v>30</v>
+      <c r="F2" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -771,8 +771,8 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>30</v>
+      <c r="F11" s="6" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
changes to written stuff for front page of website
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/cde73a511afdd567/Documents/GitHub/Pres-Inaug-Project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackg\Desktop\Pres-Inaug-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{D5B4D661-F7B3-224A-8047-6913DF175298}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{116A98A1-4FEB-4249-97DE-973ADE9F66AE}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00759D1-8B4A-463D-B97D-BA919D17E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -150,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -187,6 +187,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -208,7 +215,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -224,6 +231,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -540,23 +550,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="I21" sqref="I21"/>
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="7.69921875" customWidth="1"/>
-    <col min="2" max="2" width="8.69921875" customWidth="1"/>
-    <col min="3" max="3" width="17.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.296875" customWidth="1"/>
+    <col min="1" max="1" width="7.6640625" customWidth="1"/>
+    <col min="2" max="2" width="8.6640625" customWidth="1"/>
+    <col min="3" max="3" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.33203125" customWidth="1"/>
     <col min="6" max="6" width="14" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>28</v>
       </c>
@@ -576,7 +585,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -596,7 +605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -616,7 +625,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -636,7 +645,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -656,7 +665,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -676,7 +685,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -696,7 +705,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -716,7 +725,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -736,7 +745,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -756,7 +765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -776,7 +785,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -796,7 +805,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -812,11 +821,11 @@
       <c r="E13" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F13" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -836,7 +845,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -856,7 +865,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>15</v>
       </c>
@@ -876,7 +885,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -896,7 +905,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -916,7 +925,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>18</v>
       </c>
@@ -936,7 +945,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -956,7 +965,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -976,7 +985,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>21</v>
       </c>
@@ -996,7 +1005,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1016,7 +1025,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1036,7 +1045,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="25" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1056,7 +1065,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1076,7 +1085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1096,7 +1105,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="28" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1112,11 +1121,11 @@
       <c r="E28" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+      <c r="F28" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1136,7 +1145,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1156,7 +1165,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="31" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1176,7 +1185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1196,7 +1205,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1216,7 +1225,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="34" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1236,7 +1245,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1256,7 +1265,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1276,7 +1285,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:6" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1292,18 +1301,12 @@
       <c r="E37" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>32</v>
+      <c r="F37" s="7" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
-    <filterColumn colId="4">
-      <filters>
-        <filter val="Preetam"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:F37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
changes to excel and xml of jacks presidents
</commit_message>
<xml_diff>
--- a/Team Roles.xlsx
+++ b/Team Roles.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jackg\Desktop\Pres-Inaug-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00759D1-8B4A-463D-B97D-BA919D17E04F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2FCD330-A66E-49ED-91AE-70C3EDB7BD2F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{7EE72846-32B2-FA4F-942E-A4AC999FAD54}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="34">
   <si>
     <t>Term</t>
   </si>
@@ -135,9 +135,6 @@
   </si>
   <si>
     <t>Sworn in</t>
-  </si>
-  <si>
-    <t>In Document</t>
   </si>
   <si>
     <t>Tentative</t>
@@ -215,15 +212,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -550,10 +544,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -585,7 +580,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -601,11 +596,11 @@
       <c r="E2" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F2" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -621,7 +616,7 @@
       <c r="E3" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -641,11 +636,11 @@
       <c r="E4" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F4" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -661,11 +656,11 @@
       <c r="E5" t="s">
         <v>5</v>
       </c>
-      <c r="F5" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F5" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -681,8 +676,8 @@
       <c r="E6" t="s">
         <v>6</v>
       </c>
-      <c r="F6" s="6" t="s">
-        <v>33</v>
+      <c r="F6" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.35">
@@ -701,11 +696,11 @@
       <c r="E7" t="s">
         <v>7</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F7" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -721,11 +716,11 @@
       <c r="E8" t="s">
         <v>5</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -741,7 +736,7 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="4" t="s">
+      <c r="F9" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -761,11 +756,11 @@
       <c r="E10" t="s">
         <v>7</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F10" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -781,11 +776,11 @@
       <c r="E11" t="s">
         <v>5</v>
       </c>
-      <c r="F11" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F11" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -801,8 +796,8 @@
       <c r="E12" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="6" t="s">
-        <v>33</v>
+      <c r="F12" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.35">
@@ -821,11 +816,11 @@
       <c r="E13" t="s">
         <v>7</v>
       </c>
-      <c r="F13" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F13" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>13</v>
       </c>
@@ -841,11 +836,11 @@
       <c r="E14" t="s">
         <v>5</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>14</v>
       </c>
@@ -861,8 +856,8 @@
       <c r="E15" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>33</v>
+      <c r="F15" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.35">
@@ -881,11 +876,11 @@
       <c r="E16" t="s">
         <v>7</v>
       </c>
-      <c r="F16" s="4" t="s">
+      <c r="F16" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>16</v>
       </c>
@@ -901,11 +896,11 @@
       <c r="E17" t="s">
         <v>5</v>
       </c>
-      <c r="F17" s="5" t="s">
+      <c r="F17" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>17</v>
       </c>
@@ -921,8 +916,8 @@
       <c r="E18" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="6" t="s">
-        <v>33</v>
+      <c r="F18" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.35">
@@ -941,11 +936,11 @@
       <c r="E19" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F19" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>19</v>
       </c>
@@ -961,11 +956,11 @@
       <c r="E20" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F20" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>20</v>
       </c>
@@ -981,7 +976,7 @@
       <c r="E21" t="s">
         <v>6</v>
       </c>
-      <c r="F21" s="4" t="s">
+      <c r="F21" s="3" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1001,11 +996,11 @@
       <c r="E22" t="s">
         <v>7</v>
       </c>
-      <c r="F22" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F22" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1021,11 +1016,11 @@
       <c r="E23" t="s">
         <v>5</v>
       </c>
-      <c r="F23" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F23" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1041,8 +1036,8 @@
       <c r="E24" t="s">
         <v>6</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>33</v>
+      <c r="F24" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.35">
@@ -1061,11 +1056,11 @@
       <c r="E25" t="s">
         <v>7</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="3" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1081,11 +1076,11 @@
       <c r="E26" t="s">
         <v>5</v>
       </c>
-      <c r="F26" s="5" t="s">
+      <c r="F26" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1101,8 +1096,8 @@
       <c r="E27" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="6" t="s">
-        <v>33</v>
+      <c r="F27" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.35">
@@ -1121,11 +1116,11 @@
       <c r="E28" t="s">
         <v>7</v>
       </c>
-      <c r="F28" s="7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F28" s="6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1133,7 +1128,7 @@
         <v>1989</v>
       </c>
       <c r="C29" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29">
         <v>1</v>
@@ -1141,11 +1136,11 @@
       <c r="E29" t="s">
         <v>5</v>
       </c>
-      <c r="F29" s="5" t="s">
+      <c r="F29" s="4" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1161,8 +1156,8 @@
       <c r="E30" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="6" t="s">
-        <v>33</v>
+      <c r="F30" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.35">
@@ -1181,11 +1176,11 @@
       <c r="E31" t="s">
         <v>7</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F31" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1201,11 +1196,11 @@
       <c r="E32" t="s">
         <v>5</v>
       </c>
-      <c r="F32" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F32" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1221,8 +1216,8 @@
       <c r="E33" t="s">
         <v>6</v>
       </c>
-      <c r="F33" s="6" t="s">
-        <v>33</v>
+      <c r="F33" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.35">
@@ -1241,11 +1236,11 @@
       <c r="E34" t="s">
         <v>7</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F34" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1261,11 +1256,11 @@
       <c r="E35" t="s">
         <v>5</v>
       </c>
-      <c r="F35" s="6" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="F35" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1281,8 +1276,8 @@
       <c r="E36" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="6" t="s">
-        <v>33</v>
+      <c r="F36" s="5" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.35">
@@ -1301,12 +1296,18 @@
       <c r="E37" t="s">
         <v>7</v>
       </c>
-      <c r="F37" s="7" t="s">
-        <v>33</v>
+      <c r="F37" s="6" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}"/>
+  <autoFilter ref="A1:F37" xr:uid="{C1797F41-B8BE-5742-8ADD-0FFE7E9C715B}">
+    <filterColumn colId="4">
+      <filters>
+        <filter val="Jack"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>